<commit_message>
Correccion de subida de archivos
</commit_message>
<xml_diff>
--- a/KLS_WEB/KLS_WEB/wwwroot/Resources/LayoutOferta/CargaExcel.xlsx
+++ b/KLS_WEB/KLS_WEB/wwwroot/Resources/LayoutOferta/CargaExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consiss\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consiss\Documents\DOCS\KLS\DESARROLLO\KLS_WEB\KLS_WEB\wwwroot\Resources\LayoutOferta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03FD1DA-90AC-4126-A641-AB6A129E76D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FE3A70-1873-4A29-8540-BAE5AA08BB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C87B962D-F912-40DF-8B16-B9F069A2EB6C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Transportista</t>
   </si>
@@ -91,12 +91,6 @@
   </si>
   <si>
     <t>region</t>
-  </si>
-  <si>
-    <t>IdServiceTypes</t>
-  </si>
-  <si>
-    <t>Terrestre nacional</t>
   </si>
   <si>
     <t>GRUPO TRANSPORTES MONTERREY</t>
@@ -466,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54197AF2-5939-4FA5-806E-6199EB1CBEFF}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,11 +482,10 @@
     <col min="12" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" customWidth="1"/>
-    <col min="18" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,18 +532,15 @@
         <v>7</v>
       </c>
       <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -591,19 +581,16 @@
       <c r="O2">
         <v>56</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -644,19 +631,16 @@
       <c r="O3">
         <v>56</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -697,12 +681,12 @@
       <c r="O4">
         <v>56</v>
       </c>
-      <c r="Q4">
+      <c r="P4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q5" s="1"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>